<commit_message>
Added country to the data details
</commit_message>
<xml_diff>
--- a/outputs/Internal Fill Rate Monthly 2025-01-01 to 2025-04-30.xlsx
+++ b/outputs/Internal Fill Rate Monthly 2025-01-01 to 2025-04-30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://regalrexnord-my.sharepoint.com/personal/jenna_eagleson_regalrexnord_com/Documents/Documents/2025/2025_Core Value Drivers_Reporting/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_E6ED4C6A4E12076FD5D03E2EAFA2FCABDAB67605" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F73D527C-47E2-46DE-94D9-FAF5493C3C5C}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_E6ED4C6A4E12076FD5D03E2EAFA2FCABDAB67605" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF779127-DE0E-4A81-AADC-6C8760985DEC}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enterprise" sheetId="1" r:id="rId1"/>
@@ -3607,7 +3607,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:E29" totalsRowShown="0">
-  <autoFilter ref="A1:E29" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <autoFilter ref="A1:E29" xr:uid="{00000000-0009-0000-0100-000004000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Automation and Motion Control (AMC)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="segment_function"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="month"/>
@@ -3621,7 +3627,13 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:F183" totalsRowShown="0">
-  <autoFilter ref="A1:F183" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <autoFilter ref="A1:F183" xr:uid="{00000000-0009-0000-0100-000005000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="AMC Autonomous Mobile Solutions Division"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="segment_function"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="division_function"/>
@@ -4183,7 +4195,7 @@
         <v>0.53569999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4200,7 +4212,7 @@
         <v>0.42859999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4217,7 +4229,7 @@
         <v>0.53849999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4251,7 +4263,7 @@
         <v>0.62960000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4285,7 +4297,7 @@
         <v>0.54049999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4319,7 +4331,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4336,7 +4348,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4353,7 +4365,7 @@
         <v>0.55559999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -4387,7 +4399,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -4404,7 +4416,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4421,7 +4433,7 @@
         <v>0.41670000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -4455,7 +4467,7 @@
         <v>0.62860000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -4472,7 +4484,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -4489,7 +4501,7 @@
         <v>0.54259999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -4523,7 +4535,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -4540,7 +4552,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -4557,7 +4569,7 @@
         <v>0.41670000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -4591,7 +4603,7 @@
         <v>0.63333333333333297</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -4608,7 +4620,7 @@
         <v>0.46153846153846201</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -4625,7 +4637,7 @@
         <v>0.51694915254237295</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -4655,7 +4667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F183"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -4679,7 +4691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4719,7 +4731,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4739,7 +4751,7 @@
         <v>0.71430000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4759,7 +4771,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4779,7 +4791,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4799,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4819,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4839,7 +4851,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -4859,7 +4871,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4879,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -4899,7 +4911,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4919,7 +4931,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4939,7 +4951,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -4959,7 +4971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -4979,7 +4991,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -4999,7 +5011,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -5019,7 +5031,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -5039,7 +5051,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -5059,7 +5071,7 @@
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -5079,7 +5091,7 @@
         <v>0.68420000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -5099,7 +5111,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -5119,7 +5131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -5139,7 +5151,7 @@
         <v>0.16669999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -5159,7 +5171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -5179,7 +5191,7 @@
         <v>0.85709999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -5199,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -5239,7 +5251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -5259,7 +5271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -5279,7 +5291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -5299,7 +5311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -5319,7 +5331,7 @@
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -5339,7 +5351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -5359,7 +5371,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -5379,7 +5391,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -5399,7 +5411,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -5419,7 +5431,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -5439,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -5459,7 +5471,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -5479,7 +5491,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -5499,7 +5511,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -5519,7 +5531,7 @@
         <v>0.54549999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -5539,7 +5551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -5559,7 +5571,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -5579,7 +5591,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -5599,7 +5611,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -5619,7 +5631,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -5639,7 +5651,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -5659,7 +5671,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -5679,7 +5691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -5699,7 +5711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -5719,7 +5731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -5759,7 +5771,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -5779,7 +5791,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -5799,7 +5811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -5819,7 +5831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -5839,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -5859,7 +5871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -5879,7 +5891,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -5899,7 +5911,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -5919,7 +5931,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -5939,7 +5951,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -5959,7 +5971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -5979,7 +5991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -5999,7 +6011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -6019,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -6039,7 +6051,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -6059,7 +6071,7 @@
         <v>0.57140000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -6079,7 +6091,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -6099,7 +6111,7 @@
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -6119,7 +6131,7 @@
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -6139,7 +6151,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -6159,7 +6171,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -6179,7 +6191,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -6199,7 +6211,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -6219,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -6239,7 +6251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -6279,7 +6291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -6299,7 +6311,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -6319,7 +6331,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -6339,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -6359,7 +6371,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -6379,7 +6391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -6399,7 +6411,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -6419,7 +6431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -6439,7 +6451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>13</v>
       </c>
@@ -6459,7 +6471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -6479,7 +6491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -6499,7 +6511,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>13</v>
       </c>
@@ -6519,7 +6531,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -6539,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -6559,7 +6571,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -6579,7 +6591,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -6599,7 +6611,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -6619,7 +6631,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -6639,7 +6651,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -6659,7 +6671,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -6679,7 +6691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -6699,7 +6711,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -6719,7 +6731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -6739,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -6759,7 +6771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -6799,7 +6811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -6819,7 +6831,7 @@
         <v>0.4667</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -6839,7 +6851,7 @@
         <v>0.83330000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -6859,7 +6871,7 @@
         <v>0.85709999999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -6879,7 +6891,7 @@
         <v>0.85709999999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>12</v>
       </c>
@@ -6899,7 +6911,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -6919,7 +6931,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -6939,7 +6951,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -6959,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -6979,7 +6991,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -6999,7 +7011,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -7019,7 +7031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>13</v>
       </c>
@@ -7039,7 +7051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -7059,7 +7071,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>14</v>
       </c>
@@ -7079,7 +7091,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -7099,7 +7111,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>14</v>
       </c>
@@ -7119,7 +7131,7 @@
         <v>0.58330000000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -7139,7 +7151,7 @@
         <v>0.57140000000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>14</v>
       </c>
@@ -7159,7 +7171,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -7179,7 +7191,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -7199,7 +7211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>15</v>
       </c>
@@ -7219,7 +7231,7 @@
         <v>0.23080000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>15</v>
       </c>
@@ -7239,7 +7251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -7259,7 +7271,7 @@
         <v>0.63639999999999997</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>15</v>
       </c>
@@ -7279,7 +7291,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>12</v>
       </c>
@@ -7319,7 +7331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>12</v>
       </c>
@@ -7339,7 +7351,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>12</v>
       </c>
@@ -7359,7 +7371,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>12</v>
       </c>
@@ -7379,7 +7391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>12</v>
       </c>
@@ -7399,7 +7411,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>12</v>
       </c>
@@ -7419,7 +7431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>12</v>
       </c>
@@ -7439,7 +7451,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -7459,7 +7471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -7479,7 +7491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -7499,7 +7511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -7519,7 +7531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -7539,7 +7551,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>13</v>
       </c>
@@ -7559,7 +7571,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>13</v>
       </c>
@@ -7579,7 +7591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>14</v>
       </c>
@@ -7599,7 +7611,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>14</v>
       </c>
@@ -7619,7 +7631,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>14</v>
       </c>
@@ -7639,7 +7651,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>14</v>
       </c>
@@ -7659,7 +7671,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>14</v>
       </c>
@@ -7679,7 +7691,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>15</v>
       </c>
@@ -7699,7 +7711,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>15</v>
       </c>
@@ -7719,7 +7731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>15</v>
       </c>
@@ -7739,7 +7751,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>15</v>
       </c>
@@ -7759,7 +7771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>15</v>
       </c>
@@ -7779,7 +7791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>15</v>
       </c>
@@ -7799,7 +7811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>12</v>
       </c>
@@ -7839,7 +7851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>12</v>
       </c>
@@ -7859,7 +7871,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>12</v>
       </c>
@@ -7879,7 +7891,7 @@
         <v>0.73333333333333295</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>12</v>
       </c>
@@ -7899,7 +7911,7 @@
         <v>0.88888888888888895</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>12</v>
       </c>
@@ -7919,7 +7931,7 @@
         <v>0.84210526315789502</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>12</v>
       </c>
@@ -7939,7 +7951,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>12</v>
       </c>
@@ -7959,7 +7971,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>13</v>
       </c>
@@ -7979,7 +7991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>13</v>
       </c>
@@ -7999,7 +8011,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>13</v>
       </c>
@@ -8019,7 +8031,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>13</v>
       </c>
@@ -8039,7 +8051,7 @@
         <v>0.28571428571428598</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>13</v>
       </c>
@@ -8059,7 +8071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>13</v>
       </c>
@@ -8079,7 +8091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>13</v>
       </c>
@@ -8099,7 +8111,7 @@
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>14</v>
       </c>
@@ -8119,7 +8131,7 @@
         <v>0.41666666666666702</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>14</v>
       </c>
@@ -8139,7 +8151,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>14</v>
       </c>
@@ -8159,7 +8171,7 @@
         <v>0.52941176470588203</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>14</v>
       </c>
@@ -8179,7 +8191,7 @@
         <v>0.52941176470588203</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>14</v>
       </c>
@@ -8199,7 +8211,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>15</v>
       </c>
@@ -8219,7 +8231,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>15</v>
       </c>
@@ -8239,7 +8251,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>15</v>
       </c>
@@ -8259,7 +8271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>15</v>
       </c>
@@ -8279,7 +8291,7 @@
         <v>0.22222222222222199</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>15</v>
       </c>
@@ -8299,7 +8311,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>15</v>
       </c>
@@ -40361,7 +40373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Y284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>